<commit_message>
- protocol document updated, new command for adding AP SSID and password is added
</commit_message>
<xml_diff>
--- a/obd-charger-cmdset.xlsx
+++ b/obd-charger-cmdset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Sandbox\obd2-dongle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\sandbox\mukund\esp32-obd2-dongle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3429F51B-BB7B-49A1-9544-A4BE23F7BB54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2535" windowWidth="21600" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRAME TYPES" sheetId="7" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="263">
   <si>
     <t>Command</t>
   </si>
@@ -796,12 +797,36 @@
   </si>
   <si>
     <t>Name in ascii bytes</t>
+  </si>
+  <si>
+    <t>SETSTASSID</t>
+  </si>
+  <si>
+    <t>SETSTAPASS</t>
+  </si>
+  <si>
+    <t>Set AP SSID for dongle in STA mode</t>
+  </si>
+  <si>
+    <t>Set AP Password for dongle in STA mode</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>0x01 + len of the name including NULL character</t>
+  </si>
+  <si>
+    <t>Name in ascii bytes + NULL Character</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1015,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1114,10 +1139,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,6 +1193,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1135,25 +1211,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1165,57 +1247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1529,7 +1561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1547,20 +1579,20 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="42"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="O2" s="30" t="s">
         <v>197</v>
       </c>
@@ -1572,20 +1604,20 @@
       <c r="A3" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1600,13 +1632,13 @@
       <c r="D4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1621,13 +1653,13 @@
       <c r="D5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1642,13 +1674,13 @@
       <c r="D6" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1663,13 +1695,13 @@
       <c r="D7" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1684,13 +1716,13 @@
       <c r="D8" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1705,13 +1737,13 @@
       <c r="D9" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
@@ -1720,16 +1752,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:I6"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1737,11 +1769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,8 +1784,8 @@
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1775,24 +1807,24 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="59" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1813,10 +1845,10 @@
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1829,10 +1861,10 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="59" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1861,8 +1893,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1877,208 +1909,208 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="59"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="59"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="59"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="59"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="59"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="59"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="59"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="59"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="59"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="59"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="2">
         <v>10</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="59"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="2">
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="59"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="45"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="2" t="s">
         <v>50</v>
       </c>
@@ -2100,10 +2132,10 @@
       <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
@@ -2119,10 +2151,10 @@
       <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="59" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2137,31 +2169,31 @@
       <c r="F24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="71" t="s">
+      <c r="G24" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="71" t="s">
+      <c r="H24" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="I24" s="69" t="s">
+      <c r="I24" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="K24" s="52" t="s">
+      <c r="K24" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="L24" s="52" t="s">
+      <c r="L24" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="M24" s="52" t="s">
+      <c r="M24" s="57" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="2" t="s">
         <v>57</v>
       </c>
@@ -2174,69 +2206,69 @@
       <c r="F25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="45"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="2" t="s">
         <v>200</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="71" t="s">
+      <c r="G26" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="71" t="s">
+      <c r="H26" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I26" s="69" t="s">
+      <c r="I26" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
       <c r="E27" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="2" t="s">
         <v>11</v>
       </c>
@@ -2252,10 +2284,10 @@
       <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="59" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2270,31 +2302,31 @@
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="71" t="s">
+      <c r="G29" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="I29" s="69" t="s">
+      <c r="I29" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="J29" s="52" t="s">
+      <c r="J29" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="K29" s="52" t="s">
+      <c r="K29" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="L29" s="52" t="s">
+      <c r="L29" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="52" t="s">
+      <c r="M29" s="57" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
@@ -2307,38 +2339,38 @@
       <c r="F30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
     </row>
     <row r="31" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="45"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="29" t="s">
         <v>200</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="71" t="s">
+      <c r="G31" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H31" s="71" t="s">
+      <c r="H31" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I31" s="69" t="s">
+      <c r="I31" s="53" t="s">
         <v>150</v>
       </c>
       <c r="J31" s="14"/>
@@ -2347,29 +2379,29 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
       <c r="E32" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="70"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="54"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
       <c r="E33" s="2" t="s">
         <v>11</v>
       </c>
@@ -2385,16 +2417,16 @@
       <c r="M33" s="14"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="59" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="29" t="s">
@@ -2403,16 +2435,16 @@
       <c r="F34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="71" t="s">
+      <c r="G34" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H34" s="71" t="s">
+      <c r="H34" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="69" t="s">
+      <c r="I34" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="J34" s="55" t="s">
+      <c r="J34" s="47" t="s">
         <v>153</v>
       </c>
       <c r="K34" s="14"/>
@@ -2420,48 +2452,48 @@
       <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="55"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="47"/>
       <c r="K35" s="14"/>
       <c r="L35" s="14"/>
       <c r="M35" s="14"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="45"/>
+      <c r="D36" s="59"/>
       <c r="E36" s="29" t="s">
         <v>202</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G36" s="71" t="s">
+      <c r="G36" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H36" s="71" t="s">
+      <c r="H36" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I36" s="69" t="s">
+      <c r="I36" s="53" t="s">
         <v>152</v>
       </c>
       <c r="K36" s="14"/>
@@ -2469,34 +2501,34 @@
       <c r="M36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
       <c r="E37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="70"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="54"/>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="45" t="s">
+      <c r="C38" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="45" t="s">
+      <c r="D38" s="59" t="s">
         <v>76</v>
       </c>
       <c r="E38" s="29" t="s">
@@ -2505,94 +2537,94 @@
       <c r="F38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="71" t="s">
+      <c r="G38" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H38" s="71" t="s">
+      <c r="H38" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="I38" s="69" t="s">
+      <c r="I38" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="J38" s="55" t="s">
+      <c r="J38" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="K38" s="54"/>
+      <c r="K38" s="55"/>
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
       <c r="E39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="54"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="55"/>
       <c r="L39" s="14"/>
       <c r="M39" s="14"/>
     </row>
     <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="45"/>
+      <c r="D40" s="59"/>
       <c r="E40" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G40" s="71" t="s">
+      <c r="G40" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H40" s="71" t="s">
+      <c r="H40" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I40" s="69" t="s">
+      <c r="I40" s="53" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
       <c r="E41" s="29" t="s">
         <v>204</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="70"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="45" t="s">
+      <c r="B42" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="59" t="s">
         <v>83</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -2601,88 +2633,88 @@
       <c r="F42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="71" t="s">
+      <c r="G42" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="I42" s="69" t="s">
+      <c r="I42" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="55" t="s">
+      <c r="J42" s="47" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
+      <c r="A43" s="64"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
       <c r="E43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="72"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="55"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="47"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="45"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G44" s="71" t="s">
+      <c r="G44" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="71" t="s">
+      <c r="H44" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I44" s="69" t="s">
+      <c r="I44" s="53" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
+      <c r="A45" s="65"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="29" t="s">
         <v>204</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="70"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="45" t="s">
+      <c r="D46" s="59" t="s">
         <v>83</v>
       </c>
       <c r="E46" s="29" t="s">
@@ -2691,174 +2723,174 @@
       <c r="F46" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="71" t="s">
+      <c r="G46" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H46" s="71" t="s">
+      <c r="H46" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="I46" s="69" t="s">
+      <c r="I46" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="J46" s="55" t="s">
+      <c r="J46" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="K46" s="55" t="s">
+      <c r="K46" s="47" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="72"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
     </row>
     <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="45" t="s">
+      <c r="B48" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="45" t="s">
+      <c r="C48" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="45"/>
+      <c r="D48" s="59"/>
       <c r="E48" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="71" t="s">
+      <c r="G48" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H48" s="71" t="s">
+      <c r="H48" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I48" s="69" t="s">
+      <c r="I48" s="53" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
       <c r="E49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="72"/>
-      <c r="H49" s="72"/>
-      <c r="I49" s="70"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="45" t="s">
+      <c r="B50" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="45"/>
+      <c r="D50" s="59"/>
       <c r="E50" s="29" t="s">
         <v>203</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G50" s="71" t="s">
+      <c r="G50" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="71" t="s">
+      <c r="H50" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I50" s="69" t="s">
+      <c r="I50" s="53" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
       <c r="E51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="70"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="54"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="45" t="s">
+      <c r="B52" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="45"/>
+      <c r="D52" s="59"/>
       <c r="E52" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G52" s="71" t="s">
+      <c r="G52" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="I52" s="69" t="s">
+      <c r="I52" s="53" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G53" s="72"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="70"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="54"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="45" t="s">
+      <c r="C54" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="45" t="s">
+      <c r="D54" s="59" t="s">
         <v>104</v>
       </c>
       <c r="E54" s="29" t="s">
@@ -2867,34 +2899,34 @@
       <c r="F54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G54" s="71" t="s">
+      <c r="G54" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="H54" s="71" t="s">
+      <c r="H54" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="I54" s="69" t="s">
+      <c r="I54" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="J54" s="55" t="s">
+      <c r="J54" s="47" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
       <c r="E55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G55" s="72"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="70"/>
-      <c r="J55" s="55"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="54"/>
+      <c r="J55" s="47"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
@@ -2974,28 +3006,190 @@
       <c r="I58" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="J58" s="68" t="s">
+      <c r="J58" s="44" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+    <row r="59" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I59" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="J59" s="44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I60" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="J60" s="44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B61" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="J61" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="133">
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A21"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="E6:E21"/>
+    <mergeCell ref="F6:F21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
     <mergeCell ref="K46:K47"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G54:G55"/>
@@ -3020,115 +3214,6 @@
     <mergeCell ref="I46:I47"/>
     <mergeCell ref="J34:J35"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A21"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="E6:E21"/>
-    <mergeCell ref="F6:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3136,7 +3221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3651,7 +3736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -3671,20 +3756,20 @@
       <c r="A1" s="20"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -3692,15 +3777,15 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
@@ -3715,12 +3800,12 @@
       <c r="F4" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="74"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -3737,12 +3822,12 @@
       <c r="F5" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -3756,13 +3841,13 @@
       <c r="E6" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="74"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
@@ -3774,13 +3859,13 @@
       <c r="E7" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="67"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="74"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
@@ -3792,13 +3877,13 @@
       <c r="E8" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="67"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="74"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
@@ -3810,13 +3895,13 @@
       <c r="E9" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="72" t="s">
         <v>221</v>
       </c>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="67"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="74"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
@@ -3825,265 +3910,272 @@
       <c r="D11" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="69" t="s">
         <v>222</v>
       </c>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="64"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="71"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="66" t="s">
         <v>227</v>
       </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="F14" s="59"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="66" t="s">
         <v>230</v>
       </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
     </row>
     <row r="17" spans="3:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="57"/>
+      <c r="D18" s="76"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="56"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="75"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="75" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="75"/>
     </row>
     <row r="27" spans="3:19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="3:19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D23:S23"/>
+    <mergeCell ref="D24:S24"/>
+    <mergeCell ref="D22:S22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="D19:S19"/>
+    <mergeCell ref="D21:S21"/>
+    <mergeCell ref="D20:S20"/>
     <mergeCell ref="E16:P16"/>
     <mergeCell ref="E15:P15"/>
     <mergeCell ref="D3:J3"/>
@@ -4098,13 +4190,6 @@
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="E14:P14"/>
-    <mergeCell ref="D23:S23"/>
-    <mergeCell ref="D24:S24"/>
-    <mergeCell ref="D22:S22"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="D19:S19"/>
-    <mergeCell ref="D21:S21"/>
-    <mergeCell ref="D20:S20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- protocol sheet updated
</commit_message>
<xml_diff>
--- a/obd-charger-cmdset.xlsx
+++ b/obd-charger-cmdset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\sandbox\mukund\esp32-obd2-dongle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Sandbox\esp32-obd2-dongle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3429F51B-BB7B-49A1-9544-A4BE23F7BB54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76A2FCE-E406-4C27-A817-C762AD64F63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="264">
   <si>
     <t>Command</t>
   </si>
@@ -820,7 +820,14 @@
     <t>0x01 + len of the name including NULL character</t>
   </si>
   <si>
-    <t>Name in ascii bytes + NULL Character</t>
+    <t>Idx(1B) + Name in ascii bytes + NULL Character
+Idx - 0 (Default SSID)
+Idx - 1 (User SSID)</t>
+  </si>
+  <si>
+    <t>Idx(1B) + Name in ascii bytes + NULL Character
+Idx - 0 (Default Pass)
+Idx - 1 (User Pass)</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1148,10 +1155,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1166,50 +1219,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1238,19 +1255,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1568,7 +1578,7 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
@@ -1632,13 +1642,13 @@
       <c r="D4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="47" t="s">
         <v>241</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1653,13 +1663,13 @@
       <c r="D5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1674,13 +1684,13 @@
       <c r="D6" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1695,13 +1705,13 @@
       <c r="D7" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1716,13 +1726,13 @@
       <c r="D8" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1737,13 +1747,13 @@
       <c r="D9" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
@@ -1752,16 +1762,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:I3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1772,11 +1782,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="D56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -1785,7 +1795,7 @@
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1807,24 +1817,24 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="49" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1845,10 +1855,10 @@
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1861,10 +1871,10 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1893,8 +1903,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1909,208 +1919,208 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="59"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="49"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="59"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="59"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="49"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="59"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="59"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="59"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="59"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="49"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="59"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="59"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="59"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="59"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="59"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="49"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="59"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="59"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="59"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="49"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="2">
         <v>10</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="59"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="2">
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="59"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="59"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="2" t="s">
         <v>50</v>
       </c>
@@ -2132,10 +2142,10 @@
       <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
@@ -2151,10 +2161,10 @@
       <c r="M23" s="14"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="49" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2169,31 +2179,31 @@
       <c r="F24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="51" t="s">
+      <c r="G24" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="51" t="s">
+      <c r="H24" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="I24" s="53" t="s">
+      <c r="I24" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="57" t="s">
+      <c r="J24" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K24" s="57" t="s">
+      <c r="K24" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="L24" s="57" t="s">
+      <c r="L24" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="M24" s="57" t="s">
+      <c r="M24" s="60" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="2" t="s">
         <v>57</v>
       </c>
@@ -2206,69 +2216,69 @@
       <c r="F25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="2" t="s">
         <v>200</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="51" t="s">
+      <c r="G26" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="51" t="s">
+      <c r="H26" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I26" s="53" t="s">
+      <c r="I26" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="2" t="s">
         <v>11</v>
       </c>
@@ -2284,10 +2294,10 @@
       <c r="M28" s="14"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
+      <c r="A29" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="49" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2302,31 +2312,31 @@
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="51" t="s">
+      <c r="G29" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H29" s="51" t="s">
+      <c r="H29" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="I29" s="53" t="s">
+      <c r="I29" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="J29" s="57" t="s">
+      <c r="J29" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K29" s="57" t="s">
+      <c r="K29" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="L29" s="57" t="s">
+      <c r="L29" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="57" t="s">
+      <c r="M29" s="60" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="58"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
@@ -2339,38 +2349,38 @@
       <c r="F30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
     </row>
     <row r="31" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="59"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="29" t="s">
         <v>200</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="51" t="s">
+      <c r="G31" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H31" s="51" t="s">
+      <c r="H31" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I31" s="53" t="s">
+      <c r="I31" s="58" t="s">
         <v>150</v>
       </c>
       <c r="J31" s="14"/>
@@ -2379,29 +2389,29 @@
       <c r="M31" s="14"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="54"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="2" t="s">
         <v>11</v>
       </c>
@@ -2417,16 +2427,16 @@
       <c r="M33" s="14"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="59" t="s">
+      <c r="D34" s="49" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="29" t="s">
@@ -2435,16 +2445,16 @@
       <c r="F34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="51" t="s">
+      <c r="G34" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H34" s="51" t="s">
+      <c r="H34" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="53" t="s">
+      <c r="I34" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="63" t="s">
         <v>153</v>
       </c>
       <c r="K34" s="14"/>
@@ -2452,48 +2462,48 @@
       <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="58"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="47"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="63"/>
       <c r="K35" s="14"/>
       <c r="L35" s="14"/>
       <c r="M35" s="14"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="59"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="29" t="s">
         <v>202</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G36" s="51" t="s">
+      <c r="G36" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H36" s="51" t="s">
+      <c r="H36" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="58" t="s">
         <v>152</v>
       </c>
       <c r="K36" s="14"/>
@@ -2501,34 +2511,34 @@
       <c r="M36" s="14"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="58"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="54"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="59"/>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="59" t="s">
+      <c r="B38" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="59" t="s">
+      <c r="C38" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="49" t="s">
         <v>76</v>
       </c>
       <c r="E38" s="29" t="s">
@@ -2537,94 +2547,94 @@
       <c r="F38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H38" s="51" t="s">
+      <c r="H38" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="I38" s="53" t="s">
+      <c r="I38" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="J38" s="47" t="s">
+      <c r="J38" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="K38" s="55"/>
+      <c r="K38" s="62"/>
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="58"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
       <c r="E39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="55"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="62"/>
       <c r="L39" s="14"/>
       <c r="M39" s="14"/>
     </row>
     <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="59"/>
+      <c r="D40" s="49"/>
       <c r="E40" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G40" s="51" t="s">
+      <c r="G40" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H40" s="51" t="s">
+      <c r="H40" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I40" s="53" t="s">
+      <c r="I40" s="58" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
       <c r="E41" s="29" t="s">
         <v>204</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="54"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="63" t="s">
+      <c r="A42" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="59" t="s">
+      <c r="B42" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D42" s="59" t="s">
+      <c r="D42" s="49" t="s">
         <v>83</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -2633,88 +2643,88 @@
       <c r="F42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="51" t="s">
+      <c r="G42" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H42" s="51" t="s">
+      <c r="H42" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="I42" s="53" t="s">
+      <c r="I42" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="47" t="s">
+      <c r="J42" s="63" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="64"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="59"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
       <c r="E43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="47"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="59"/>
+      <c r="D44" s="49"/>
       <c r="E44" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G44" s="51" t="s">
+      <c r="G44" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="51" t="s">
+      <c r="H44" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I44" s="53" t="s">
+      <c r="I44" s="58" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
       <c r="E45" s="29" t="s">
         <v>204</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="54"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="59"/>
     </row>
     <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="59" t="s">
+      <c r="D46" s="49" t="s">
         <v>83</v>
       </c>
       <c r="E46" s="29" t="s">
@@ -2723,174 +2733,174 @@
       <c r="F46" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G46" s="51" t="s">
+      <c r="G46" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H46" s="51" t="s">
+      <c r="H46" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="I46" s="53" t="s">
+      <c r="I46" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="J46" s="47" t="s">
+      <c r="J46" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="K46" s="47" t="s">
+      <c r="K46" s="63" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="58"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
       <c r="E47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
     </row>
     <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="58" t="s">
+      <c r="A48" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="59" t="s">
+      <c r="C48" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="59"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I48" s="53" t="s">
+      <c r="I48" s="58" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
       <c r="E49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="54"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="59"/>
     </row>
     <row r="50" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="59" t="s">
+      <c r="C50" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="59"/>
+      <c r="D50" s="49"/>
       <c r="E50" s="29" t="s">
         <v>203</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G50" s="51" t="s">
+      <c r="G50" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="51" t="s">
+      <c r="H50" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I50" s="53" t="s">
+      <c r="I50" s="58" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="58"/>
-      <c r="B51" s="59"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
+      <c r="A51" s="48"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
       <c r="E51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="54"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="59"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="59" t="s">
+      <c r="B52" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="59"/>
+      <c r="D52" s="49"/>
       <c r="E52" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G52" s="51" t="s">
+      <c r="G52" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H52" s="51" t="s">
+      <c r="H52" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="I52" s="53" t="s">
+      <c r="I52" s="58" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="58"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
+      <c r="A53" s="48"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G53" s="52"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="54"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="59"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="58" t="s">
+      <c r="A54" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="59" t="s">
+      <c r="B54" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="59" t="s">
+      <c r="D54" s="49" t="s">
         <v>104</v>
       </c>
       <c r="E54" s="29" t="s">
@@ -2899,34 +2909,34 @@
       <c r="F54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G54" s="51" t="s">
+      <c r="G54" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="H54" s="51" t="s">
+      <c r="H54" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="I54" s="53" t="s">
+      <c r="I54" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="J54" s="47" t="s">
+      <c r="J54" s="63" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="58"/>
-      <c r="B55" s="59"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
       <c r="E55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G55" s="52"/>
-      <c r="H55" s="52"/>
-      <c r="I55" s="54"/>
-      <c r="J55" s="47"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="63"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
@@ -3010,7 +3020,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="42" t="s">
         <v>255</v>
       </c>
@@ -3032,11 +3042,11 @@
       <c r="I59" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="J59" s="44" t="s">
+      <c r="J59" s="79" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="42" t="s">
         <v>256</v>
       </c>
@@ -3058,8 +3068,8 @@
       <c r="I60" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="J60" s="44" t="s">
-        <v>262</v>
+      <c r="J60" s="79" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3077,119 +3087,10 @@
       <c r="F61" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="J61" s="78"/>
+      <c r="J61" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="133">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A21"/>
-    <mergeCell ref="B4:B21"/>
-    <mergeCell ref="E6:E21"/>
-    <mergeCell ref="F6:F21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
     <mergeCell ref="K46:K47"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G54:G55"/>
@@ -3214,6 +3115,115 @@
     <mergeCell ref="I46:I47"/>
     <mergeCell ref="J34:J35"/>
     <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A21"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="E6:E21"/>
+    <mergeCell ref="F6:F21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3228,7 +3238,7 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
@@ -3743,7 +3753,7 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -3756,20 +3766,20 @@
       <c r="A1" s="20"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -3777,15 +3787,15 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
@@ -3800,12 +3810,12 @@
       <c r="F4" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="74"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -3822,12 +3832,12 @@
       <c r="F5" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -3841,13 +3851,13 @@
       <c r="E6" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="74"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
@@ -3859,13 +3869,13 @@
       <c r="E7" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="74"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
@@ -3877,13 +3887,13 @@
       <c r="E8" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="74"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="78"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
@@ -3895,13 +3905,13 @@
       <c r="E9" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="74"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="78"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
@@ -3910,272 +3920,265 @@
       <c r="D11" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="71"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="75"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="70" t="s">
         <v>228</v>
       </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="71"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="70" t="s">
         <v>229</v>
       </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="67"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="71"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="70" t="s">
         <v>230</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
-      <c r="P15" s="67"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="71"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="E16" s="66" t="s">
+      <c r="E16" s="70" t="s">
         <v>231</v>
       </c>
-      <c r="F16" s="66"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
-      <c r="P16" s="67"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
     </row>
     <row r="17" spans="3:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="76"/>
+      <c r="D18" s="68"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="69" t="s">
         <v>211</v>
       </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="75"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="75" t="s">
+      <c r="D21" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="75"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="75" t="s">
+      <c r="D22" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75"/>
-      <c r="S22" s="75"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D23" s="75" t="s">
+      <c r="D23" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
-      <c r="S23" s="75"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
     </row>
     <row r="27" spans="3:19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="3:19" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D23:S23"/>
-    <mergeCell ref="D24:S24"/>
-    <mergeCell ref="D22:S22"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="D19:S19"/>
-    <mergeCell ref="D21:S21"/>
-    <mergeCell ref="D20:S20"/>
     <mergeCell ref="E16:P16"/>
     <mergeCell ref="E15:P15"/>
     <mergeCell ref="D3:J3"/>
@@ -4190,6 +4193,13 @@
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="E14:P14"/>
+    <mergeCell ref="D23:S23"/>
+    <mergeCell ref="D24:S24"/>
+    <mergeCell ref="D22:S22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="D19:S19"/>
+    <mergeCell ref="D21:S21"/>
+    <mergeCell ref="D20:S20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>